<commit_message>
update name of build-in resources
</commit_message>
<xml_diff>
--- a/data/country/v1.xlsx
+++ b/data/country/v1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/rd/project/zentao/go/zd/data/country/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AF453F-8584-8C49-96C4-9DCA488C2822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6253EB1B-3783-9345-94F6-D701608369C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4880" yWindow="460" windowWidth="23420" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="country" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4385,7 +4385,7 @@
   <dimension ref="A1:IT206"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>

</xml_diff>